<commit_message>
Added in ppt and modified excel sheet and plots
</commit_message>
<xml_diff>
--- a/data/Zooplankton-species-counts-bamfield2022.xlsx
+++ b/data/Zooplankton-species-counts-bamfield2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ar/Desktop/eosc573/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ar/Desktop/School:work/GradSchool/Year 1/Courses/EOSC573/Project/eosc573/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FAF7C6-DE06-424E-AF3F-A141569A918F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BA65BB-700C-1549-830E-33DE775A73A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="460" windowWidth="22400" windowHeight="16680" activeTab="4" xr2:uid="{0D48336A-9344-BE4D-81A2-EFF2F9B1002C}"/>
+    <workbookView xWindow="6120" yWindow="460" windowWidth="22400" windowHeight="16680" activeTab="3" xr2:uid="{0D48336A-9344-BE4D-81A2-EFF2F9B1002C}"/>
   </bookViews>
   <sheets>
     <sheet name="Species counts" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="282">
   <si>
     <t>Zoplankton data sheet</t>
   </si>
@@ -942,6 +942,9 @@
   <si>
     <t>Paracalanus/Clausocalanus</t>
   </si>
+  <si>
+    <t>Aerial biomass (mgC/m^2)</t>
+  </si>
 </sst>
 </file>
 
@@ -1276,7 +1279,6 @@
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1284,8 +1286,9 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3581,7 +3584,7 @@
             <c:numRef>
               <c:f>'Size structure'!$L$5:$O$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>15.86826347</c:v>
@@ -3652,7 +3655,7 @@
             <c:numRef>
               <c:f>'Size structure'!$L$6:$O$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>33.233532930000003</c:v>
@@ -3723,7 +3726,7 @@
             <c:numRef>
               <c:f>'Size structure'!$L$7:$O$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>41.616766470000002</c:v>
@@ -3794,7 +3797,7 @@
             <c:numRef>
               <c:f>'Size structure'!$L$8:$O$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5.9880239519999998</c:v>
@@ -3865,7 +3868,7 @@
             <c:numRef>
               <c:f>'Size structure'!$L$9:$O$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2.0958083830000001</c:v>
@@ -3973,7 +3976,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -10571,6 +10574,36 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -10583,11 +10616,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Biomass!$K$37</c:f>
+              <c:f>Biomass!$K$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Biomass w euphausiids</c:v>
+                  <c:v>Aerial biomass (mgC/m^2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10624,21 +10657,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Biomass!$L$37:$O$37</c:f>
+              <c:f>Biomass!$L$39:$O$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.5895861314436068</c:v>
+                  <c:v>167.6875839433082</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.251322865390399</c:v>
+                  <c:v>787.53968596171194</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2491141734378606</c:v>
+                  <c:v>194.94685040627164</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.078325850135119</c:v>
+                  <c:v>3369.3991020162143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10646,77 +10679,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-800D-3843-9E9F-59AC7503DA69}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Biomass!$K$38</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Biomass w/o euphausiids</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Biomass!$L$36:$O$36</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>SR</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>N1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>D2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>D1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Biomass!$L$38:$O$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5.5895861314436068</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.271515837490902</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.2491141734378606</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.704614874559347</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-800D-3843-9E9F-59AC7503DA69}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10848,37 +10810,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -17760,16 +17691,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>226985</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>5437</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>36485</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>170537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>744969</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>137384</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>554469</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>365984</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17796,16 +17727,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>787890</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>21002</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>567197</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>111649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>388942</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>120511</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>69779</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>71642</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17833,15 +17764,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>57898</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:colOff>468780</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>178548</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>485590</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>168089</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>74707</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>112060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28383,8 +28314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4179ED0C-29BF-004B-A242-993B295C52C4}">
   <dimension ref="A1:AI39"/>
   <sheetViews>
-    <sheetView topLeftCell="J10" zoomScale="68" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView topLeftCell="F23" zoomScale="91" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30435,8 +30366,26 @@
         <v>7.704614874559347</v>
       </c>
     </row>
-    <row r="39" spans="11:15">
-      <c r="K39" s="25"/>
+    <row r="39" spans="11:15" ht="51">
+      <c r="K39" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="L39">
+        <f>L37*30</f>
+        <v>167.6875839433082</v>
+      </c>
+      <c r="M39">
+        <f>M37*30</f>
+        <v>787.53968596171194</v>
+      </c>
+      <c r="N39">
+        <f>N37*60</f>
+        <v>194.94685040627164</v>
+      </c>
+      <c r="O39">
+        <f>O37*120</f>
+        <v>3369.3991020162143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30449,8 +30398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F79EF9-D9D4-FC4F-A9A1-1A9C4BD5E74C}">
   <dimension ref="B2:V58"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="50" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30461,6 +30410,8 @@
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="35" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
     <col min="16" max="16" width="14.33203125" customWidth="1"/>
   </cols>
@@ -30529,16 +30480,16 @@
       <c r="K5" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="L5" s="45">
+      <c r="L5" s="54">
         <v>15.86826347</v>
       </c>
-      <c r="M5" s="45">
+      <c r="M5" s="54">
         <v>45.42533873</v>
       </c>
-      <c r="N5" s="45">
+      <c r="N5" s="54">
         <v>38.933333330000004</v>
       </c>
-      <c r="O5" s="45">
+      <c r="O5" s="54">
         <v>7.6484947109999997</v>
       </c>
     </row>
@@ -30555,16 +30506,16 @@
       <c r="K6" s="44" t="s">
         <v>264</v>
       </c>
-      <c r="L6" s="45">
+      <c r="L6" s="54">
         <v>33.233532930000003</v>
       </c>
-      <c r="M6" s="45">
+      <c r="M6" s="54">
         <v>17.600223490000001</v>
       </c>
-      <c r="N6" s="45">
+      <c r="N6" s="54">
         <v>21.2991274</v>
       </c>
-      <c r="O6" s="45">
+      <c r="O6" s="54">
         <v>24.89829129</v>
       </c>
     </row>
@@ -30581,16 +30532,16 @@
       <c r="K7" s="44" t="s">
         <v>265</v>
       </c>
-      <c r="L7" s="45">
+      <c r="L7" s="54">
         <v>41.616766470000002</v>
       </c>
-      <c r="M7" s="45">
+      <c r="M7" s="54">
         <v>30.507054060000002</v>
       </c>
-      <c r="N7" s="45">
+      <c r="N7" s="54">
         <v>32.266666669999999</v>
       </c>
-      <c r="O7" s="45">
+      <c r="O7" s="54">
         <v>20.341741249999998</v>
       </c>
     </row>
@@ -30607,16 +30558,16 @@
       <c r="K8" s="44" t="s">
         <v>267</v>
       </c>
-      <c r="L8" s="45">
+      <c r="L8" s="54">
         <v>5.9880239519999998</v>
       </c>
-      <c r="M8" s="45">
+      <c r="M8" s="54">
         <v>4.1905294040000003</v>
       </c>
-      <c r="N8" s="45">
+      <c r="N8" s="54">
         <v>7.733333333</v>
       </c>
-      <c r="O8" s="45">
+      <c r="O8" s="54">
         <v>40.856387310000002</v>
       </c>
     </row>
@@ -30633,16 +30584,16 @@
       <c r="K9" s="44" t="s">
         <v>269</v>
       </c>
-      <c r="L9" s="45">
+      <c r="L9" s="54">
         <v>2.0958083830000001</v>
       </c>
-      <c r="M9" s="45">
+      <c r="M9" s="54">
         <v>0.41207311600000002</v>
       </c>
-      <c r="N9" s="45">
+      <c r="N9" s="54">
         <v>1.066666667</v>
       </c>
-      <c r="O9" s="45">
+      <c r="O9" s="54">
         <v>4.6277461349999998</v>
       </c>
       <c r="R9" s="24"/>
@@ -31558,7 +31509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F97DE8-FE64-144B-8488-623DC1DF8D57}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -32169,65 +32120,65 @@
       <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="46"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="53"/>
       <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="50" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="49" t="s">
         <v>276</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="48">
         <v>2.2389210632570999</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="48">
         <v>0.79024090012639703</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="48">
         <v>1.8876183539467499</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="48">
         <v>0.65307113134841299</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="48">
         <v>2.1494813620790398</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="48">
         <v>0.73001389306683795</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="48">
         <v>2.4981034801973498</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="48">
         <v>0.79671761711640798</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="47"/>
+      <c r="A8" s="46"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="19"/>
@@ -32263,7 +32214,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="31">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>278</v>
       </c>
     </row>

</xml_diff>